<commit_message>
Parser: Introduced SLR(1) parser
Parser is capable of producing a complete syntax tree for cases that are already covered. This tree will be converted to script instructions later. When that happens, this SLR(1) parser will become official, and its output will be used in script execution. Currently, generated syntax tree is not used, but simply discarded.
</commit_message>
<xml_diff>
--- a/Script Grammar.xlsx
+++ b/Script Grammar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\live-coder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639C156A-986B-4C16-B811-6AB46C2F09CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5EEC61-9631-46F0-8CCE-E9BE458BF703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{15C34A51-DAD1-4386-9970-F050F5750DAB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="146">
   <si>
     <t>S' -&gt; S</t>
   </si>
@@ -295,9 +295,6 @@
   </si>
   <si>
     <t>L -&gt; .R*</t>
-  </si>
-  <si>
-    <t>Shift ., 14</t>
   </si>
   <si>
     <t>Reduce 8</t>
@@ -1420,7 +1417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDF57F7-A307-416F-8837-DF478C82AE5A}">
   <dimension ref="B1:AA63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1448,7 +1447,7 @@
       <c r="I2" s="78"/>
       <c r="J2" s="79"/>
       <c r="L2" s="69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M2" s="70"/>
       <c r="N2" s="70"/>
@@ -1496,19 +1495,19 @@
         <v>25</v>
       </c>
       <c r="O3" s="40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q3" s="40" t="s">
         <v>36</v>
       </c>
       <c r="R3" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="S3" s="40" t="s">
         <v>118</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>119</v>
       </c>
       <c r="T3" s="41" t="s">
         <v>35</v>
@@ -1532,7 +1531,7 @@
         <v>33</v>
       </c>
       <c r="AA3" s="66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
@@ -1559,19 +1558,19 @@
         <v>0</v>
       </c>
       <c r="M4" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O4" s="43"/>
       <c r="P4" s="43"/>
       <c r="Q4" s="43"/>
       <c r="R4" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="S4" s="43" t="s">
         <v>122</v>
-      </c>
-      <c r="S4" s="43" t="s">
-        <v>123</v>
       </c>
       <c r="T4" s="44"/>
       <c r="U4" s="45">
@@ -1593,7 +1592,7 @@
         <v>8</v>
       </c>
       <c r="AA4" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
@@ -1620,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N5" s="48"/>
       <c r="O5" s="48"/>
@@ -1629,7 +1628,7 @@
       <c r="R5" s="48"/>
       <c r="S5" s="48"/>
       <c r="T5" s="49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U5" s="50"/>
       <c r="V5" s="51">
@@ -1667,7 +1666,7 @@
         <v>2</v>
       </c>
       <c r="M6" s="60" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N6" s="48"/>
       <c r="O6" s="48"/>
@@ -1676,7 +1675,7 @@
       <c r="R6" s="48"/>
       <c r="S6" s="48"/>
       <c r="T6" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U6" s="50"/>
       <c r="V6" s="51"/>
@@ -1710,10 +1709,10 @@
         <v>3</v>
       </c>
       <c r="M7" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N7" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O7" s="48"/>
       <c r="P7" s="48"/>
@@ -1721,7 +1720,7 @@
       <c r="R7" s="48"/>
       <c r="S7" s="48"/>
       <c r="T7" s="49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U7" s="50"/>
       <c r="V7" s="51"/>
@@ -1748,7 +1747,7 @@
         <v>45</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>62</v>
@@ -1757,7 +1756,7 @@
         <v>4</v>
       </c>
       <c r="M8" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N8" s="48"/>
       <c r="O8" s="48"/>
@@ -1791,7 +1790,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>64</v>
@@ -1801,7 +1800,7 @@
       </c>
       <c r="M9" s="60"/>
       <c r="N9" s="48" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="O9" s="48"/>
       <c r="P9" s="48"/>
@@ -1832,7 +1831,7 @@
         <v>47</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>66</v>
@@ -1841,20 +1840,20 @@
         <v>6</v>
       </c>
       <c r="M10" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O10" s="48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P10" s="48"/>
       <c r="Q10" s="48"/>
       <c r="R10" s="48"/>
       <c r="S10" s="48"/>
       <c r="T10" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U10" s="50"/>
       <c r="V10" s="51"/>
@@ -1876,7 +1875,7 @@
         <v>48</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>66</v>
@@ -1888,10 +1887,10 @@
       <c r="N11" s="48"/>
       <c r="O11" s="48"/>
       <c r="P11" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q11" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R11" s="48"/>
       <c r="S11" s="48"/>
@@ -1916,7 +1915,7 @@
         <v>49</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>66</v>
@@ -1928,7 +1927,7 @@
       <c r="N12" s="48"/>
       <c r="O12" s="48"/>
       <c r="P12" s="48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q12" s="48"/>
       <c r="R12" s="48"/>
@@ -1966,10 +1965,10 @@
       <c r="N13" s="48"/>
       <c r="O13" s="48"/>
       <c r="P13" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q13" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R13" s="48"/>
       <c r="S13" s="48"/>
@@ -2006,10 +2005,10 @@
       <c r="N14" s="48"/>
       <c r="O14" s="48"/>
       <c r="P14" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q14" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R14" s="48"/>
       <c r="S14" s="48"/>
@@ -2043,7 +2042,7 @@
         <v>11</v>
       </c>
       <c r="M15" s="60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N15" s="48"/>
       <c r="O15" s="48"/>
@@ -2052,7 +2051,7 @@
       <c r="R15" s="48"/>
       <c r="S15" s="48"/>
       <c r="T15" s="49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U15" s="50"/>
       <c r="V15" s="51"/>
@@ -2083,10 +2082,10 @@
         <v>12</v>
       </c>
       <c r="M16" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N16" s="48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O16" s="48"/>
       <c r="P16" s="48"/>
@@ -2094,7 +2093,7 @@
       <c r="R16" s="48"/>
       <c r="S16" s="48"/>
       <c r="T16" s="49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U16" s="50"/>
       <c r="V16" s="51"/>
@@ -2121,10 +2120,10 @@
         <v>13</v>
       </c>
       <c r="M17" s="60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N17" s="48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O17" s="48"/>
       <c r="P17" s="48"/>
@@ -2132,7 +2131,7 @@
       <c r="R17" s="48"/>
       <c r="S17" s="48"/>
       <c r="T17" s="49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U17" s="50"/>
       <c r="V17" s="51"/>
@@ -2165,13 +2164,13 @@
       <c r="O18" s="48"/>
       <c r="P18" s="48"/>
       <c r="Q18" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R18" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="S18" s="48" t="s">
         <v>122</v>
-      </c>
-      <c r="S18" s="48" t="s">
-        <v>123</v>
       </c>
       <c r="T18" s="49"/>
       <c r="U18" s="50"/>
@@ -2212,10 +2211,10 @@
       <c r="P19" s="48"/>
       <c r="Q19" s="48"/>
       <c r="R19" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="S19" s="48" t="s">
         <v>122</v>
-      </c>
-      <c r="S19" s="48" t="s">
-        <v>123</v>
       </c>
       <c r="T19" s="49"/>
       <c r="U19" s="50"/>
@@ -2249,7 +2248,7 @@
         <v>16</v>
       </c>
       <c r="M20" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N20" s="48"/>
       <c r="O20" s="48"/>
@@ -2280,7 +2279,7 @@
         <v>47</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J21" s="21" t="s">
         <v>66</v>
@@ -2289,10 +2288,10 @@
         <v>17</v>
       </c>
       <c r="M21" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N21" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O21" s="48"/>
       <c r="P21" s="48"/>
@@ -2300,7 +2299,7 @@
       <c r="R21" s="48"/>
       <c r="S21" s="48"/>
       <c r="T21" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U21" s="50"/>
       <c r="V21" s="51"/>
@@ -2322,7 +2321,7 @@
         <v>48</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J22" s="21" t="s">
         <v>66</v>
@@ -2334,10 +2333,10 @@
       <c r="N22" s="48"/>
       <c r="O22" s="48"/>
       <c r="P22" s="48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R22" s="48"/>
       <c r="S22" s="48"/>
@@ -2362,7 +2361,7 @@
         <v>49</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J23" s="21" t="s">
         <v>66</v>
@@ -2374,10 +2373,10 @@
       <c r="N23" s="48"/>
       <c r="O23" s="48"/>
       <c r="P23" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q23" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R23" s="48"/>
       <c r="S23" s="48"/>
@@ -2413,7 +2412,7 @@
         <v>20</v>
       </c>
       <c r="M24" s="60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N24" s="48"/>
       <c r="O24" s="48"/>
@@ -2422,7 +2421,7 @@
       <c r="R24" s="48"/>
       <c r="S24" s="48"/>
       <c r="T24" s="49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U24" s="50"/>
       <c r="V24" s="51"/>
@@ -2449,10 +2448,10 @@
         <v>21</v>
       </c>
       <c r="M25" s="61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N25" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O25" s="54"/>
       <c r="P25" s="54"/>
@@ -2460,7 +2459,7 @@
       <c r="R25" s="54"/>
       <c r="S25" s="54"/>
       <c r="T25" s="55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U25" s="56"/>
       <c r="V25" s="57"/>
@@ -2527,7 +2526,7 @@
         <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G29" s="34">
         <v>4</v>
@@ -2536,7 +2535,7 @@
         <v>63</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>86</v>
@@ -2547,14 +2546,14 @@
         <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G30" s="35"/>
       <c r="H30" s="7" t="s">
         <v>47</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>66</v>
@@ -2572,7 +2571,7 @@
         <v>48</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>66</v>
@@ -2590,7 +2589,7 @@
         <v>49</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>66</v>
@@ -2604,10 +2603,10 @@
         <v>65</v>
       </c>
       <c r="I33" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J33" s="30" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
@@ -2618,10 +2617,10 @@
         <v>67</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="7:10" x14ac:dyDescent="0.25">
@@ -2630,10 +2629,10 @@
         <v>68</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2642,10 +2641,10 @@
         <v>69</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2659,7 +2658,7 @@
         <v>37</v>
       </c>
       <c r="J37" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2673,7 +2672,7 @@
         <v>37</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2687,7 +2686,7 @@
         <v>37</v>
       </c>
       <c r="J39" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2701,7 +2700,7 @@
         <v>37</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2729,7 +2728,7 @@
         <v>38</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2741,7 +2740,7 @@
         <v>38</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2752,10 +2751,10 @@
         <v>87</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="7:10" x14ac:dyDescent="0.25">
@@ -2763,25 +2762,25 @@
         <v>14</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G46" s="14"/>
       <c r="H46" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="7:10" x14ac:dyDescent="0.25">
@@ -2805,7 +2804,7 @@
         <v>37</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
@@ -2837,13 +2836,13 @@
         <v>15</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>37</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.25">
@@ -2875,13 +2874,13 @@
         <v>16</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I54" s="17" t="s">
         <v>38</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="7:10" x14ac:dyDescent="0.25">
@@ -2925,13 +2924,13 @@
         <v>17</v>
       </c>
       <c r="H58" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I58" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="7:10" x14ac:dyDescent="0.25">
@@ -2939,13 +2938,13 @@
         <v>18</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2954,10 +2953,10 @@
         <v>75</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J60" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2965,13 +2964,13 @@
         <v>19</v>
       </c>
       <c r="H61" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I61" s="26" t="s">
         <v>37</v>
       </c>
       <c r="J61" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2979,13 +2978,13 @@
         <v>20</v>
       </c>
       <c r="H62" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I62" s="29" t="s">
         <v>38</v>
       </c>
       <c r="J62" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2993,13 +2992,13 @@
         <v>21</v>
       </c>
       <c r="H63" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I63" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J63" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parser: Added tests for syntax tree generator
</commit_message>
<xml_diff>
--- a/Script Grammar.xlsx
+++ b/Script Grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\live-coder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5EEC61-9631-46F0-8CCE-E9BE458BF703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47FD15C-B266-4956-8DA2-6A237E952059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{15C34A51-DAD1-4386-9970-F050F5750DAB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="146">
   <si>
     <t>S' -&gt; S</t>
   </si>
@@ -1417,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDF57F7-A307-416F-8837-DF478C82AE5A}">
   <dimension ref="B1:AA63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2414,9 @@
       <c r="M24" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="N24" s="48"/>
+      <c r="N24" s="48" t="s">
+        <v>129</v>
+      </c>
       <c r="O24" s="48"/>
       <c r="P24" s="48"/>
       <c r="Q24" s="48"/>
@@ -2877,7 +2879,7 @@
         <v>99</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="J54" s="18" t="s">
         <v>107</v>
@@ -2889,7 +2891,7 @@
         <v>47</v>
       </c>
       <c r="I55" s="20" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="J55" s="21" t="s">
         <v>66</v>
@@ -2901,7 +2903,7 @@
         <v>48</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="J56" s="21" t="s">
         <v>66</v>
@@ -2913,7 +2915,7 @@
         <v>49</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="J57" s="24" t="s">
         <v>66</v>
@@ -2981,7 +2983,7 @@
         <v>108</v>
       </c>
       <c r="I62" s="29" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="J62" s="30" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Added "Command" to the command class's name to easier spot it
</commit_message>
<xml_diff>
--- a/Script Grammar.xlsx
+++ b/Script Grammar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\live-coder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47FD15C-B266-4956-8DA2-6A237E952059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F5DA9-30A0-4C81-A75C-D27F917487EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{15C34A51-DAD1-4386-9970-F050F5750DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{15C34A51-DAD1-4386-9970-F050F5750DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Grammar" sheetId="1" r:id="rId1"/>
@@ -1417,9 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDF57F7-A307-416F-8837-DF478C82AE5A}">
   <dimension ref="B1:AA63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>